<commit_message>
feat: add data filtering options and Excel report generation functionality
</commit_message>
<xml_diff>
--- a/static/parte-template.xlsx
+++ b/static/parte-template.xlsx
@@ -12,7 +12,7 @@
     <sheet name="CAUSA" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'PARTE DEPTOS'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'PARTE DEPTOS'!$A$1:$I$17</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">${Destino}</t>
   </si>
@@ -35,6 +35,9 @@
     <t xml:space="preserve">FECHA</t>
   </si>
   <si>
+    <t xml:space="preserve">${fecha}</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nombre</t>
   </si>
   <si>
@@ -60,21 +63,6 @@
   </si>
   <si>
     <t xml:space="preserve">OBSERVACIONES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${table:Marcadas.Nombre}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${table:Marcadas.MR}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${table:Marcadas.CUIL}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${table:Marcadas.Salida}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${table:Marcadas.Entrada}</t>
   </si>
   <si>
     <t xml:space="preserve">FE PERMANENTE </t>
@@ -231,7 +219,7 @@
     <numFmt numFmtId="166" formatCode="m/d/yyyy\ h:mm"/>
     <numFmt numFmtId="167" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,12 +310,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -490,7 +472,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -615,62 +597,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -687,7 +613,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="6" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="6" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -899,22 +825,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="21.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="24.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16381" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -929,6 +857,8 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -947,9 +877,8 @@
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="n">
-        <f aca="true">TODAY()</f>
-        <v>45736</v>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
@@ -972,57 +901,47 @@
     </row>
     <row r="5" s="13" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
     </row>
     <row r="6" s="13" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>16</v>
-      </c>
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="J6" s="0"/>
+      <c r="K6" s="0"/>
     </row>
     <row r="7" s="13" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="16"/>
@@ -1034,13 +953,15 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
     </row>
     <row r="8" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="8"/>
@@ -1049,13 +970,15 @@
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
       <c r="I8" s="21"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
     </row>
     <row r="9" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="8"/>
@@ -1064,13 +987,15 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="21"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
     </row>
     <row r="10" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="25" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="15"/>
@@ -1079,6 +1004,8 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="21"/>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0"/>
     </row>
     <row r="11" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="21"/>
@@ -1090,10 +1017,12 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="21"/>
+      <c r="J11" s="0"/>
+      <c r="K11" s="0"/>
     </row>
     <row r="12" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -1103,6 +1032,8 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
     </row>
     <row r="13" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
@@ -1114,361 +1045,60 @@
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="8"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
     </row>
     <row r="14" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="21"/>
       <c r="E14" s="21"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="27"/>
       <c r="I14" s="5"/>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
     </row>
     <row r="15" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="21"/>
+      <c r="D15" s="28"/>
       <c r="E15" s="21"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
-      <c r="H15" s="27"/>
+      <c r="H15" s="15"/>
       <c r="I15" s="5"/>
-    </row>
-    <row r="16" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="15"/>
+      <c r="J15" s="0"/>
+      <c r="K15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="28"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="28"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="21"/>
+      <c r="E17" s="29"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="30"/>
-    </row>
-    <row r="21" s="13" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="22" s="13" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="15"/>
-    </row>
-    <row r="23" s="13" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="34"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-    </row>
-    <row r="24" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="34"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="37"/>
-    </row>
-    <row r="25" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="41"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-    </row>
-    <row r="26" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E26" s="34"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="31"/>
-    </row>
-    <row r="27" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="43"/>
-    </row>
-    <row r="28" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="34"/>
-    </row>
-    <row r="32" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="44"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="42"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I34" s="13"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I35" s="13"/>
-    </row>
-    <row r="36" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="2"/>
-    </row>
-    <row r="38" s="13" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" s="13" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1"/>
-      <c r="C40" s="2"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="13"/>
-      <c r="I41" s="13"/>
-    </row>
-    <row r="42" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1"/>
-      <c r="C42" s="2"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-    </row>
-    <row r="43" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="2"/>
-    </row>
-    <row r="44" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1"/>
-      <c r="C44" s="2"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-    </row>
-    <row r="45" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="2"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="13"/>
-    </row>
-    <row r="46" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="2"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="13"/>
-    </row>
-    <row r="47" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1"/>
-      <c r="C47" s="2"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-    </row>
-    <row r="48" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1"/>
-      <c r="C48" s="2"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-    </row>
-    <row r="49" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1"/>
-      <c r="C49" s="2"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-    </row>
-    <row r="50" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1"/>
-      <c r="C50" s="2"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="34"/>
-      <c r="I51" s="34"/>
-    </row>
-    <row r="52" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1"/>
-      <c r="C52" s="2"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-    </row>
-    <row r="53" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="2"/>
-    </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="34"/>
-      <c r="I54" s="34"/>
-    </row>
-    <row r="55" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1"/>
-      <c r="C55" s="2"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-    </row>
-    <row r="56" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="2"/>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="34"/>
-      <c r="I57" s="34"/>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="34"/>
-      <c r="I58" s="34"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1496,203 +1126,203 @@
       <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="71.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="45" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="71.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="31" width="11.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="46" t="s">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="46" t="s">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="46" t="s">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="46" t="s">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="46" t="s">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="46" t="s">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="46" t="s">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="32" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="46" t="s">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="46" t="s">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="46" t="s">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="46" t="s">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="32" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="46" t="s">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="32" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="46" t="s">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="32" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="46" t="s">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="46" t="s">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="46" t="s">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="46" t="s">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="46" t="s">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="32" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="47" t="s">
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="46" t="s">
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="32" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="46" t="s">
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="32" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="46" t="s">
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="46" t="s">
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="46" t="s">
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="32" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="46" t="s">
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="32" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="46" t="s">
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="32" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="46" t="s">
+      <c r="B32" s="31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="46" t="s">
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="32" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="46" t="s">
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="46" t="s">
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="45" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="32" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="46" t="s">
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="34" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="46" t="s">
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="35" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="46" t="s">
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="32" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="46" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="48" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="49" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="46" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>